<commit_message>
04/01/26 New Year Push
</commit_message>
<xml_diff>
--- a/src/main/java/DataSheets/Testsheet.xlsx
+++ b/src/main/java/DataSheets/Testsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VijayBala\IdeaProject\src\main\java\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CBA41B-DECE-4187-BEF6-7C8ECDB7DF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F1188-0299-4117-821C-2AA9A809A6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Robin</t>
   </si>
@@ -126,16 +126,22 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>0d32ae3fd27814b7ab921e81ef5f8b59</t>
-  </si>
-  <si>
-    <t>4f9302e0f46baa74ebd420dd50189f6a</t>
-  </si>
-  <si>
     <t>181b7ae2882fa39f355de28be3bd073e</t>
   </si>
   <si>
     <t>ca008a7dfa37d35f5d0ada20a3321ec8</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>TestcaseID</t>
+  </si>
+  <si>
+    <t>TS01_TC01</t>
+  </si>
+  <si>
+    <t>TS02_TC01</t>
   </si>
 </sst>
 </file>
@@ -182,13 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true"/>
@@ -473,78 +478,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E4E32D-78F7-41BD-9694-11F859F0551E}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.88671875"/>
-    <col min="2" max="2" customWidth="true" width="21.33203125"/>
-    <col min="3" max="3" customWidth="true" width="22.21875"/>
-    <col min="4" max="4" customWidth="true" width="20.44140625"/>
-    <col min="5" max="5" customWidth="true" width="28.5546875"/>
+    <col min="1" max="1" customWidth="true" width="20.6640625"/>
+    <col min="2" max="2" customWidth="true" width="32.88671875"/>
+    <col min="3" max="3" customWidth="true" width="21.33203125"/>
+    <col min="4" max="4" customWidth="true" width="22.21875"/>
+    <col min="5" max="5" customWidth="true" width="20.44140625"/>
+    <col min="6" max="6" customWidth="true" width="28.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="C1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="E1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="F1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="G1" t="s" s="0">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="F2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s" s="5">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s" s="7">
+      <c r="E3" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s" s="6">
         <v>25</v>
       </c>
     </row>

</xml_diff>